<commit_message>
new results with plot
</commit_message>
<xml_diff>
--- a/results/random_queries.xlsx
+++ b/results/random_queries.xlsx
@@ -170,7 +170,7 @@
                 <c:formatCode>0.00E+00</c:formatCode>
                 <c:ptCount val="3"/>
                 <c:pt idx="0">
-                  <c:v>23652085542000</c:v>
+                  <c:v>11040057040000</c:v>
                 </c:pt>
                 <c:pt idx="1">
                   <c:v>30288191936270</c:v>
@@ -191,11 +191,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="94318592"/>
-        <c:axId val="116520000"/>
+        <c:axId val="78716928"/>
+        <c:axId val="78706880"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="94318592"/>
+        <c:axId val="78716928"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -204,7 +204,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="116520000"/>
+        <c:crossAx val="78706880"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -212,7 +212,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="116520000"/>
+        <c:axId val="78706880"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -223,7 +223,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="94318592"/>
+        <c:crossAx val="78716928"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -262,16 +262,6 @@
     <c:title>
       <c:layout/>
       <c:overlay val="0"/>
-      <c:txPr>
-        <a:bodyPr/>
-        <a:lstStyle/>
-        <a:p>
-          <a:pPr>
-            <a:defRPr sz="2000"/>
-          </a:pPr>
-          <a:endParaRPr lang="en-US"/>
-        </a:p>
-      </c:txPr>
     </c:title>
     <c:autoTitleDeleted val="0"/>
     <c:plotArea>
@@ -295,25 +285,6 @@
             </c:strRef>
           </c:tx>
           <c:invertIfNegative val="0"/>
-          <c:dLbls>
-            <c:txPr>
-              <a:bodyPr/>
-              <a:lstStyle/>
-              <a:p>
-                <a:pPr>
-                  <a:defRPr sz="1200"/>
-                </a:pPr>
-                <a:endParaRPr lang="en-US"/>
-              </a:p>
-            </c:txPr>
-            <c:showLegendKey val="0"/>
-            <c:showVal val="1"/>
-            <c:showCatName val="0"/>
-            <c:showSerName val="0"/>
-            <c:showPercent val="0"/>
-            <c:showBubbleSize val="0"/>
-            <c:showLeaderLines val="0"/>
-          </c:dLbls>
           <c:errBars>
             <c:errBarType val="both"/>
             <c:errValType val="cust"/>
@@ -325,7 +296,7 @@
                   <c:formatCode>General</c:formatCode>
                   <c:ptCount val="3"/>
                   <c:pt idx="0">
-                    <c:v>3209597237149.6865</c:v>
+                    <c:v>262908185954.42108</c:v>
                   </c:pt>
                   <c:pt idx="1">
                     <c:v>2316651061532.3716</c:v>
@@ -343,7 +314,7 @@
                   <c:formatCode>General</c:formatCode>
                   <c:ptCount val="3"/>
                   <c:pt idx="0">
-                    <c:v>3209597237149.6865</c:v>
+                    <c:v>262908185954.42108</c:v>
                   </c:pt>
                   <c:pt idx="1">
                     <c:v>2316651061532.3716</c:v>
@@ -379,7 +350,7 @@
                 <c:formatCode>0.00E+00</c:formatCode>
                 <c:ptCount val="3"/>
                 <c:pt idx="0">
-                  <c:v>23652085542000</c:v>
+                  <c:v>11040057040000</c:v>
                 </c:pt>
                 <c:pt idx="1">
                   <c:v>30288191936270</c:v>
@@ -400,11 +371,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="94319616"/>
-        <c:axId val="96760896"/>
+        <c:axId val="55590912"/>
+        <c:axId val="45768704"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="94319616"/>
+        <c:axId val="55590912"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -423,7 +394,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="96760896"/>
+        <c:crossAx val="45768704"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -431,13 +402,39 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="96760896"/>
+        <c:axId val="45768704"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="l"/>
         <c:majorGridlines/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr/>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US" sz="1800"/>
+                  <a:t>Number of Row accesses</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout>
+            <c:manualLayout>
+              <c:xMode val="edge"/>
+              <c:yMode val="edge"/>
+              <c:x val="4.5859860344755414E-2"/>
+              <c:y val="0.24314561679790025"/>
+            </c:manualLayout>
+          </c:layout>
+          <c:overlay val="0"/>
+        </c:title>
         <c:numFmt formatCode="0.00E+00" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
@@ -452,30 +449,38 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="94319616"/>
+        <c:crossAx val="55590912"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
+      <c:dTable>
+        <c:showHorzBorder val="1"/>
+        <c:showVertBorder val="1"/>
+        <c:showOutline val="1"/>
+        <c:showKeys val="1"/>
+        <c:txPr>
+          <a:bodyPr/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr rtl="0">
+              <a:defRPr sz="1400"/>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+      </c:dTable>
     </c:plotArea>
-    <c:legend>
-      <c:legendPos val="r"/>
-      <c:layout/>
-      <c:overlay val="0"/>
-      <c:txPr>
-        <a:bodyPr/>
-        <a:lstStyle/>
-        <a:p>
-          <a:pPr>
-            <a:defRPr sz="1800"/>
-          </a:pPr>
-          <a:endParaRPr lang="en-US"/>
-        </a:p>
-      </c:txPr>
-    </c:legend>
     <c:plotVisOnly val="1"/>
     <c:dispBlanksAs val="gap"/>
     <c:showDLblsOverMax val="0"/>
   </c:chart>
+  <c:spPr>
+    <a:ln w="15875">
+      <a:solidFill>
+        <a:schemeClr val="tx1"/>
+      </a:solidFill>
+    </a:ln>
+  </c:spPr>
   <c:printSettings>
     <c:headerFooter/>
     <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
@@ -873,7 +878,7 @@
   <dimension ref="A1:D22"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" zoomScaleSheetLayoutView="100" workbookViewId="0">
-      <selection activeCell="B20" sqref="B20"/>
+      <selection activeCell="F3" sqref="F3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -891,7 +896,7 @@
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B2" s="1">
-        <v>660066110000</v>
+        <v>10800055800000</v>
       </c>
       <c r="C2" s="1">
         <v>10849562640175</v>
@@ -902,7 +907,7 @@
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B3" s="1">
-        <v>38400090400000</v>
+        <v>9600049600000</v>
       </c>
       <c r="C3" s="1">
         <v>38459099510300</v>
@@ -913,7 +918,7 @@
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B4" s="1">
-        <v>19800087300000</v>
+        <v>10800055800000</v>
       </c>
       <c r="C4" s="1">
         <v>30049591140300</v>
@@ -924,7 +929,7 @@
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B5" s="1">
-        <v>39600096600000</v>
+        <v>10800055800000</v>
       </c>
       <c r="C5" s="1">
         <v>39633602860275</v>
@@ -935,7 +940,7 @@
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B6" s="1">
-        <v>19800087300000</v>
+        <v>13200068200000</v>
       </c>
       <c r="C6" s="1">
         <v>32449103530300</v>
@@ -950,7 +955,7 @@
       </c>
       <c r="B7" s="1">
         <f>AVERAGE(B2:B6)</f>
-        <v>23652085542000</v>
+        <v>11040057040000</v>
       </c>
       <c r="C7" s="1">
         <f>AVERAGE(C2:C6)</f>
@@ -967,7 +972,7 @@
       </c>
       <c r="B8">
         <f>STDEV(B2:B6)</f>
-        <v>16047986185748.432</v>
+        <v>1314540929772.1055</v>
       </c>
       <c r="C8">
         <f>STDEV(C2:C6)</f>
@@ -984,7 +989,7 @@
       </c>
       <c r="B9" s="1">
         <f>STDEV(B2:B6)/COUNT(B2:B6)</f>
-        <v>3209597237149.6865</v>
+        <v>262908185954.42108</v>
       </c>
       <c r="C9" s="1">
         <f>STDEV(C2:C6)/COUNT(C2:C6)</f>
@@ -1012,7 +1017,7 @@
       </c>
       <c r="B20" s="1">
         <f>AVERAGE(B2:B6)</f>
-        <v>23652085542000</v>
+        <v>11040057040000</v>
       </c>
       <c r="C20" s="1">
         <f>AVERAGE(C2:C6)</f>
@@ -1029,7 +1034,7 @@
       </c>
       <c r="B21">
         <f>STDEV(B2:B6)</f>
-        <v>16047986185748.432</v>
+        <v>1314540929772.1055</v>
       </c>
       <c r="C21">
         <f>STDEV(C2:C6)</f>
@@ -1046,7 +1051,7 @@
       </c>
       <c r="B22" s="1">
         <f>STDEV(B2:B6)/COUNT(B2:B6)</f>
-        <v>3209597237149.6865</v>
+        <v>262908185954.42108</v>
       </c>
       <c r="C22" s="1">
         <f>STDEV(C2:C6)/COUNT(C2:C6)</f>

</xml_diff>